<commit_message>
Reorganización de documentación del proyecto, se incluye primer prototipo base y primeras descripciones de algunos casos de uso (de Adrian Bustamate), también actualización de la 'Plantilla de Casos de Uso.xlsx'
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla de Casos de Uso.xlsx
+++ b/Plantillas/Plantilla de Casos de Uso.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\watwi\Desktop\Archivos - Desarrollo de software\plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\watwi\Desktop\Archivos - Desarrollo de software\EMA-Desarrollo-de-software-Equipo-2\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="26475" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2250" windowWidth="26475" windowHeight="14025" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -195,9 +195,6 @@
     <t>Administrar egresos</t>
   </si>
   <si>
-    <t>Recibir pago alumnos</t>
-  </si>
-  <si>
     <t>Visualizar historial de pagos de piso</t>
   </si>
   <si>
@@ -225,30 +222,18 @@
     <t>El director podrá registrar y dar de baja a alumnos del sistema, al igual que poder visualizar sus detalles.</t>
   </si>
   <si>
-    <t>Vacío</t>
-  </si>
-  <si>
     <t>El colaborador podrá tomar asistencia de los alumnos pertenecientes a un grupo.</t>
   </si>
   <si>
     <t>El director podrá visualizar y modificar horas de los grupos o rentas disponibles.</t>
   </si>
   <si>
-    <t>El colaborador podrá registrar los pagos de alumnos en el sistema.</t>
-  </si>
-  <si>
-    <t>Registrar pagos de alumnos</t>
-  </si>
-  <si>
     <t>El director podrá registrar, modificar y visualizar detalles de los clientes a los que se le ofrece el servicio de renta.</t>
   </si>
   <si>
     <t>El director podrá registrar, modificar y visualizar detalles de colaboradores.</t>
   </si>
   <si>
-    <t>El director podrá registrar pagos de los colaboradores y clientes.</t>
-  </si>
-  <si>
     <t>El colaborador podrá crear, modificar y dar de baja promociones para las inscripciones a sus respectivos grupos</t>
   </si>
   <si>
@@ -258,9 +243,6 @@
     <t>El director podra ingresar, modificar y visualizar egresos en el sistema.</t>
   </si>
   <si>
-    <t>El director podrá realizar un lista de chequeo de los alumnos de los cuales el recibió un pago para un respectivo colaborador.</t>
-  </si>
-  <si>
     <t>El colaborador podra visualizar un historial de los pagos recibidos por los alumnos en un lapso de tiempo definido.</t>
   </si>
   <si>
@@ -289,6 +271,24 @@
   </si>
   <si>
     <t xml:space="preserve"> 02:00 hrs</t>
+  </si>
+  <si>
+    <t>Administrar pagos de alumnos</t>
+  </si>
+  <si>
+    <t>El director podrá registrar pagos de los colaboradores y clientes. Pudiendo generar un recibo.</t>
+  </si>
+  <si>
+    <t>El colaborador podrá registrar y modificar los pagos de alumnos en el sistema. Pudiendo generar un recibo.</t>
+  </si>
+  <si>
+    <t>El director podrá crear o modificar un lista de chequeo de los alumnos de los cuales el recibió un pago para un respectivo colaborador.</t>
+  </si>
+  <si>
+    <t>Administrar pago a colaborador</t>
+  </si>
+  <si>
+    <t>Planificado</t>
   </si>
 </sst>
 </file>
@@ -718,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="D4" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,22 +778,22 @@
         <v>23</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I5" s="6"/>
     </row>
@@ -802,22 +802,22 @@
         <v>27</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>25</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I6" s="6"/>
     </row>
@@ -826,22 +826,22 @@
         <v>28</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>26</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I7" s="6"/>
     </row>
@@ -850,46 +850,46 @@
         <v>29</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>45</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I9" s="6"/>
     </row>
@@ -898,22 +898,22 @@
         <v>31</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>46</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I10" s="6"/>
     </row>
@@ -922,22 +922,22 @@
         <v>32</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>47</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I11" s="6"/>
     </row>
@@ -946,22 +946,22 @@
         <v>33</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>48</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I12" s="6"/>
     </row>
@@ -970,22 +970,22 @@
         <v>34</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>49</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I13" s="6"/>
     </row>
@@ -994,22 +994,22 @@
         <v>35</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>50</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I14" s="6"/>
     </row>
@@ -1018,22 +1018,22 @@
         <v>36</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>51</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I15" s="6"/>
     </row>
@@ -1042,22 +1042,22 @@
         <v>37</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I16" s="6"/>
     </row>
@@ -1066,22 +1066,22 @@
         <v>38</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I17" s="6"/>
     </row>
@@ -1090,22 +1090,22 @@
         <v>39</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I18" s="6"/>
     </row>
@@ -1114,22 +1114,22 @@
         <v>40</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I19" s="6"/>
     </row>
@@ -1138,22 +1138,22 @@
         <v>41</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I20" s="6"/>
     </row>
@@ -1162,22 +1162,22 @@
         <v>42</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I21" s="6"/>
     </row>
@@ -1186,22 +1186,22 @@
         <v>43</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I22" s="6"/>
     </row>
@@ -1210,22 +1210,22 @@
         <v>44</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I23" s="6"/>
     </row>
@@ -1243,8 +1243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C12"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Actualización de CUs y se agregan Prototipos correspondientes
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla de Casos de Uso.xlsx
+++ b/Plantillas/Plantilla de Casos de Uso.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2250" windowWidth="26475" windowHeight="14025" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3150" windowWidth="26475" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="83">
   <si>
     <t>Columna</t>
   </si>
@@ -270,9 +270,6 @@
     <t>Documento ERS</t>
   </si>
   <si>
-    <t xml:space="preserve"> 02:00 hrs</t>
-  </si>
-  <si>
     <t>Administrar pagos de alumnos</t>
   </si>
   <si>
@@ -295,7 +292,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,6 +335,14 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -394,7 +399,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -410,6 +415,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -716,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,17 +743,17 @@
     <col min="11" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
@@ -773,7 +779,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>23</v>
       </c>
@@ -784,11 +790,9 @@
         <v>24</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>77</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F5" s="8"/>
       <c r="G5" s="8" t="s">
         <v>76</v>
       </c>
@@ -797,7 +801,7 @@
       </c>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>27</v>
       </c>
@@ -808,11 +812,9 @@
         <v>25</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>77</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F6" s="8"/>
       <c r="G6" s="8" t="s">
         <v>76</v>
       </c>
@@ -821,7 +823,7 @@
       </c>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>28</v>
       </c>
@@ -832,11 +834,9 @@
         <v>26</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>77</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F7" s="8"/>
       <c r="G7" s="8" t="s">
         <v>76</v>
       </c>
@@ -845,7 +845,7 @@
       </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>29</v>
       </c>
@@ -856,11 +856,9 @@
         <v>45</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>77</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F8" s="8"/>
       <c r="G8" s="8" t="s">
         <v>76</v>
       </c>
@@ -869,22 +867,20 @@
       </c>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>77</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F9" s="8"/>
       <c r="G9" s="8" t="s">
         <v>76</v>
       </c>
@@ -893,7 +889,7 @@
       </c>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>31</v>
       </c>
@@ -904,11 +900,9 @@
         <v>46</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>77</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F10" s="8"/>
       <c r="G10" s="8" t="s">
         <v>76</v>
       </c>
@@ -917,22 +911,21 @@
       </c>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
       <c r="B11" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>47</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>77</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F11" s="8"/>
       <c r="G11" s="8" t="s">
         <v>76</v>
       </c>
@@ -941,7 +934,7 @@
       </c>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>33</v>
       </c>
@@ -952,11 +945,9 @@
         <v>48</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>77</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F12" s="8"/>
       <c r="G12" s="8" t="s">
         <v>76</v>
       </c>
@@ -965,7 +956,7 @@
       </c>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>34</v>
       </c>
@@ -976,11 +967,9 @@
         <v>49</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>77</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F13" s="8"/>
       <c r="G13" s="8" t="s">
         <v>76</v>
       </c>
@@ -989,7 +978,7 @@
       </c>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>35</v>
       </c>
@@ -1000,11 +989,9 @@
         <v>50</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>77</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F14" s="8"/>
       <c r="G14" s="8" t="s">
         <v>76</v>
       </c>
@@ -1013,7 +1000,7 @@
       </c>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>36</v>
       </c>
@@ -1024,11 +1011,9 @@
         <v>51</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>77</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F15" s="8"/>
       <c r="G15" s="8" t="s">
         <v>76</v>
       </c>
@@ -1037,22 +1022,20 @@
       </c>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C16" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>82</v>
-      </c>
       <c r="E16" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>77</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F16" s="8"/>
       <c r="G16" s="8" t="s">
         <v>76</v>
       </c>
@@ -1072,11 +1055,9 @@
         <v>52</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>77</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F17" s="8"/>
       <c r="G17" s="8" t="s">
         <v>76</v>
       </c>
@@ -1096,11 +1077,9 @@
         <v>53</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>77</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F18" s="8"/>
       <c r="G18" s="8" t="s">
         <v>76</v>
       </c>
@@ -1120,11 +1099,9 @@
         <v>54</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>77</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F19" s="8"/>
       <c r="G19" s="8" t="s">
         <v>76</v>
       </c>
@@ -1144,11 +1121,9 @@
         <v>55</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>77</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F20" s="8"/>
       <c r="G20" s="8" t="s">
         <v>76</v>
       </c>
@@ -1168,11 +1143,9 @@
         <v>56</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>77</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F21" s="8"/>
       <c r="G21" s="8" t="s">
         <v>76</v>
       </c>
@@ -1192,11 +1165,9 @@
         <v>57</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>77</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F22" s="8"/>
       <c r="G22" s="8" t="s">
         <v>76</v>
       </c>
@@ -1216,11 +1187,9 @@
         <v>58</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>77</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F23" s="8"/>
       <c r="G23" s="8" t="s">
         <v>76</v>
       </c>
@@ -1243,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A6" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>